<commit_message>
work on detecting input & keybindings
</commit_message>
<xml_diff>
--- a/Keybindings Guide.xlsx
+++ b/Keybindings Guide.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="83">
   <si>
     <t>Key ID</t>
   </si>
@@ -242,13 +242,37 @@
     <t>8, numpad 8</t>
   </si>
   <si>
-    <t>5, numpad 5</t>
-  </si>
-  <si>
     <t>4, numpad 4</t>
   </si>
   <si>
     <t>6, numpad 6</t>
+  </si>
+  <si>
+    <t>Internal Keycode</t>
+  </si>
+  <si>
+    <t>Binding Keycode</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>81, 32</t>
+  </si>
+  <si>
+    <t>56, 104</t>
+  </si>
+  <si>
+    <t>5, numpad 5, 2, numpad 2</t>
+  </si>
+  <si>
+    <t>53, 101, 50, 98</t>
+  </si>
+  <si>
+    <t>52, 100</t>
+  </si>
+  <si>
+    <t>54, 102</t>
   </si>
 </sst>
 </file>
@@ -300,12 +324,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,9 +629,11 @@
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -614,8 +646,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -628,8 +666,14 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -642,8 +686,14 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>27</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -656,8 +706,14 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>36</v>
+      </c>
+      <c r="F4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -670,8 +726,14 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -684,8 +746,14 @@
       <c r="D6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>40</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -698,8 +766,14 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>37</v>
+      </c>
+      <c r="F7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -712,8 +786,14 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -726,8 +806,14 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>87</v>
+      </c>
+      <c r="F9">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -740,8 +826,14 @@
       <c r="D10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>83</v>
+      </c>
+      <c r="F10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -754,8 +846,14 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -768,8 +866,14 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>68</v>
+      </c>
+      <c r="F12">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -782,8 +886,14 @@
       <c r="D13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>81</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -796,8 +906,14 @@
       <c r="D14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>69</v>
+      </c>
+      <c r="F14" s="5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -810,8 +926,14 @@
       <c r="D15" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>56</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -822,10 +944,16 @@
         <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="E16">
+        <v>53</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -836,10 +964,16 @@
         <v>4</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E17">
+        <v>52</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -850,10 +984,16 @@
         <v>6</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E18">
+        <v>54</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -866,8 +1006,14 @@
       <c r="D19" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>73</v>
+      </c>
+      <c r="F19">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -880,8 +1026,14 @@
       <c r="D20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>75</v>
+      </c>
+      <c r="F20">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -894,8 +1046,14 @@
       <c r="D21" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>74</v>
+      </c>
+      <c r="F21">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -908,8 +1066,14 @@
       <c r="D22" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>76</v>
+      </c>
+      <c r="F22">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -922,8 +1086,14 @@
       <c r="D23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>85</v>
+      </c>
+      <c r="F23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -935,6 +1105,12 @@
       </c>
       <c r="D24" t="s">
         <v>70</v>
+      </c>
+      <c r="E24">
+        <v>79</v>
+      </c>
+      <c r="F24">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>